<commit_message>
Change option to lack_of_power to lack_of_power_fuel
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerators/forms/refrigerator_status/refrigerator_status.xlsx
+++ b/app/config/tables/refrigerators/forms/refrigerator_status/refrigerator_status.xlsx
@@ -261,15 +261,6 @@
     <t>Investigación desconocida / de necesidades</t>
   </si>
   <si>
-    <t>lack_of_power</t>
-  </si>
-  <si>
-    <t>Lack of Power</t>
-  </si>
-  <si>
-    <t>Falta de poder</t>
-  </si>
-  <si>
     <t>awaiting_installation</t>
   </si>
   <si>
@@ -466,6 +457,15 @@
   </si>
   <si>
     <t>not_functioning</t>
+  </si>
+  <si>
+    <t>lack_of_power_fuel</t>
+  </si>
+  <si>
+    <t>Lack of Power/Fuel</t>
+  </si>
+  <si>
+    <t>Falta de poder/combustible</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>0</v>
@@ -1040,19 +1040,19 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1113,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -1122,7 +1122,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -1166,7 +1166,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -1175,7 +1175,7 @@
         <v>24</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F4" t="s">
         <v>75</v>
@@ -1195,7 +1195,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J4" t="s">
         <v>73</v>
@@ -1204,12 +1204,12 @@
         <v>26</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
@@ -1224,7 +1224,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J5" t="s">
         <v>31</v>
@@ -1233,7 +1233,7 @@
         <v>30</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>58</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J6" t="s">
         <v>59</v>
@@ -1262,7 +1262,7 @@
         <v>60</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1310,36 +1310,36 @@
         <v>7</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E3" s="30"/>
     </row>
@@ -1361,7 +1361,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1378,24 +1378,24 @@
         <v>78</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="28" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>95</v>
+      <c r="B7" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,16 +1403,16 @@
         <v>27</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,16 +1420,16 @@
         <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1437,16 +1437,16 @@
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1460,10 +1460,10 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,13 +1471,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E13" s="30"/>
     </row>
@@ -1486,13 +1486,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E14" s="30"/>
     </row>
@@ -1501,13 +1501,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E15" s="30"/>
     </row>
@@ -1516,13 +1516,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E16" s="30"/>
     </row>
@@ -1531,13 +1531,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" s="30"/>
     </row>
@@ -1555,7 +1555,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>67</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>68</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
         <v>69</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +1650,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
         <v>41</v>
@@ -1659,7 +1659,7 @@
         <v>42</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1700,10 +1700,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H5" s="16"/>
     </row>
@@ -1729,7 +1729,7 @@
         <v>51</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,22 +1744,22 @@
         <v>54</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>